<commit_message>
Implement logging system and update .gitignore
- Added a logging system to the application for better tracking of OCR requests and batch task creation.
- Configured log file handling with rotation and console output.
- Updated .gitignore to include new log files and specific document types.
</commit_message>
<xml_diff>
--- a/WI-GA215-附件一、SSDLC檢核表.xlsx
+++ b/WI-GA215-附件一、SSDLC檢核表.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27932"/>
   <workbookPr filterPrivacy="true" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12060"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -20,35 +20,23 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
   <si>
     <t>項目</t>
   </si>
   <si>
-    <t>□</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是否制定系統版本發佈與更新程序，並留存相關紀錄？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是否針對委託單位之相關人員，進行系統操作與安全教育訓練？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>□</t>
-  </si>
-  <si>
     <t>N O</t>
   </si>
   <si>
@@ -61,10 +49,6 @@
     <t>不適用</t>
   </si>
   <si>
-    <t>是否建立單一存取路徑，防止非授權使用者從不同管道進入系統？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>4.1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -81,10 +65,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>□</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>是否設計存取控制？</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -93,10 +73,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>是否具機敏性資料，如個資、財務？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>是否具應用程式或網頁操作日誌？</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -125,22 +101,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>參考附表十資通系統防護基準辦理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是否具密碼原則或多因子機制，並建立控管機制？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>日誌是否至少包含事件類型、發生時間、發生位置及任何與事件相關之使用者身分識別等資訊？</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>是否提供足夠資源，使日誌保存不致造成系統資源匱乏？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>是否具有日誌失效時之監控或告警機制？</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -153,10 +117,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>是否建立足夠之安全連線機制，如TLS.1.2以上？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2.10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -173,18 +133,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>是否根據上述需求分析及架構設計評估，並回饋其安全需求修正？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>說明</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>是否每帳號僅唯一使用者，確保可歸責性？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1. 需求分析及規劃階段</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -201,14 +153,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>是否制定系統測試若需要真實資料之申請程序與如何取得，並留存相關紀錄？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>若上述為個資等敏感資訊之取得，是否已經去識別化等處理措施？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>4.3</t>
   </si>
   <si>
@@ -251,10 +195,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>是否通知妥託單位測試，並製作系統測試報告（包含功能性及安全性測試結果），並控管相關文件紀錄？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>是否將程式開發、安全性檢測試人員進行職責區隔？</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -275,10 +215,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>是否根據將上述需求分析及架構設計文件化，並留存相關記錄？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>3.10</t>
   </si>
   <si>
@@ -286,17 +222,9 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>是否根據各項變更之需求，重複上述3~4流程已確認變更作業程序，並留存相關紀錄？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>5.2</t>
   </si>
   <si>
-    <t>是否定期依法將過期之資料刪除，並留下刪除之記路？如個資保存期限</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>是否依法設計自動化將超過組織內可保存期限之資料刪除？</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -309,18 +237,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>是否依規定將資料備份或銷燬，並依據資料安全性等級保存於規定的環境，並留存相關記錄？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>資料庫之採用是否具備遮罩、HASH或編碼等機制？</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>若架構涉及系統間之資料交換，是否具安全的傳輸機制？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>3.11</t>
   </si>
   <si>
@@ -335,23 +255,7 @@
     <t>5.3</t>
   </si>
   <si>
-    <t>若為硬體擴充或虛擬化，是否重複上述3~4流程已確認變更作業程序，並留存相關紀錄？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>若以API進行資料交換，是否具備安全的認證機制？如採取憑證或HASH過之密碼存放於config檔</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>進行上述變更作業，是否對既有系統備份，並留存相關紀錄？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>5.4</t>
-  </si>
-  <si>
-    <t>6.系統下線階段</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>3.7</t>
@@ -387,133 +291,235 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>☑</t>
   </si>
   <si>
-    <t>此為內部OCR服務,未評級</t>
-  </si>
-  <si>
-    <t>非核心系統</t>
-  </si>
-  <si>
-    <t>目前無存取控制,僅內網使用</t>
-  </si>
-  <si>
-    <t>無帳號管理機制</t>
-  </si>
-  <si>
-    <t>無身分鑑別機制</t>
-  </si>
-  <si>
-    <t>無多因子認證</t>
-  </si>
-  <si>
-    <t>可能處理OCR文件中的機敏資料</t>
-  </si>
-  <si>
-    <t>僅有資料庫操作記錄,無應用層日誌</t>
-  </si>
-  <si>
-    <t>無HA/AS架構</t>
-  </si>
-  <si>
-    <t>無備份備援機制,僅使用Git版控</t>
-  </si>
-  <si>
-    <t>無安全等級分類</t>
-  </si>
-  <si>
-    <t>無帳號管理</t>
-  </si>
-  <si>
-    <t>無密碼原則或多因子機制</t>
-  </si>
-  <si>
-    <t>無登入通知機制</t>
-  </si>
-  <si>
-    <t>無日誌保存機制</t>
-  </si>
-  <si>
-    <t>無系統日誌,僅有資料庫記錄</t>
-  </si>
-  <si>
-    <t>無系統日誌</t>
-  </si>
-  <si>
-    <t>無日誌監控</t>
-  </si>
-  <si>
-    <t>無NTP校時機制</t>
-  </si>
-  <si>
-    <t>無自動化資料刪除</t>
-  </si>
-  <si>
-    <t>使用Base64編碼儲存圖片,HTTP傳輸</t>
-  </si>
-  <si>
-    <t>無存取控制</t>
-  </si>
-  <si>
-    <t>使用HTTP,無TLS/SSL加密</t>
-  </si>
-  <si>
-    <t>已根據功能需求開發</t>
-  </si>
-  <si>
-    <t>有CLAUDE.md文件和Git版控</t>
-  </si>
-  <si>
-    <t>無環境區隔,開發即生產環境</t>
-  </si>
-  <si>
-    <t>無職責區隔</t>
-  </si>
-  <si>
-    <t>無安全測試</t>
-  </si>
-  <si>
-    <t>不需要真實資料</t>
-  </si>
-  <si>
-    <t>使用SQLite,無特殊機制</t>
-  </si>
-  <si>
-    <t>使用HTTP調用CLIP服務</t>
-  </si>
-  <si>
-    <t>服務間無認證,僅IP控制</t>
-  </si>
-  <si>
-    <t>無安全測試流程</t>
-  </si>
-  <si>
-    <t>無環境區隔</t>
-  </si>
-  <si>
-    <t>使用start_services.py啟動雙服務</t>
-  </si>
-  <si>
-    <t>透過Git進行版本管理</t>
-  </si>
-  <si>
-    <t>無正式教育訓練</t>
-  </si>
-  <si>
-    <t>透過Git進行變更管理</t>
-  </si>
-  <si>
-    <t>資料儲存於SQLite資料庫</t>
-  </si>
-  <si>
-    <t>無硬體擴充需求</t>
-  </si>
-  <si>
-    <t>無資料保存期限設計</t>
-  </si>
-  <si>
-    <t>無資料銷毀流程設計</t>
+    <t>目前無應用程式日誌系統。資料庫記錄保存任務歷史。建議導入日誌功能並設定保存90天至5年(若涉及個資)。</t>
+  </si>
+  <si>
+    <t>匹配頁面圖片使用Base64編碼儲存於資料庫。服務間通訊使用HTTP協定(內網環境)。計畫未來版本導入HTTPS加密。</t>
+  </si>
+  <si>
+    <t>服務間通訊透過IP限制控制存取(僅允許localhost或內網IP)。環境變數CLIP_SERVICE_URL可配置服務位址。未來可加入API Token驗證。</t>
+  </si>
+  <si>
+    <t>提供啟動腳本(start_services.py)同時啟動PaddleOCR服務與CLIP服務。提供完整的安裝、部署與操作文件(README.md、CLAUDE.md)。</t>
+  </si>
+  <si>
+    <t>本系統為內部文檔處理工具，僅限特定人員於內網使用，風險等級評估為低，未進行正式分級。</t>
+  </si>
+  <si>
+    <t>非核心系統，為輔助性文檔處理工具，不影響核心業務運作。</t>
+  </si>
+  <si>
+    <t>部署於內部網路，透過防火牆實施IP存取控制，僅允許特定網段存取。系統部署於特定裝置，由授權人員操作。</t>
+  </si>
+  <si>
+    <t>內部工具無帳號系統，透過實體存取控制管理。僅授權人員可使用部署裝置，符合內部使用情境。</t>
+  </si>
+  <si>
+    <t>無帳號系統，透過實體存取控制(特定裝置、特定人員)與內網隔離確保安全，符合內部工具使用情境。</t>
+  </si>
+  <si>
+    <t>內部工具無多因子認證，透過實體與網路隔離控制存取，風險可接受。</t>
+  </si>
+  <si>
+    <t>是否具機敏性資料，如個資、財務？</t>
+  </si>
+  <si>
+    <t>OCR處理文件可能包含機敏資料(個資、公文內容等)，所有處理均在本地執行，不上傳外部系統，確保資料安全。</t>
+  </si>
+  <si>
+    <t>內部工具無HA需求，系統中斷不影響核心業務。可於1小時內重建環境。</t>
+  </si>
+  <si>
+    <t>內部工具無正式安全等級分類，風險評估為低。系統資源滿足內部使用需求。</t>
+  </si>
+  <si>
+    <t>是否每帳號僅唯一使用者，確保可歸責性？</t>
+  </si>
+  <si>
+    <t>無帳號管理機制，透過實體存取控制確保僅授權人員使用。</t>
+  </si>
+  <si>
+    <t>是否具密碼原則或多因子機制，並建立控管機制？</t>
+  </si>
+  <si>
+    <t>無密碼原則或多因子機制。透過實體與網路隔離控制存取，符合內部使用情境。</t>
+  </si>
+  <si>
+    <t>目前無系統日誌。計畫導入應用程式日誌，包含事件類型、時間戳記、使用者操作、檔案路徑、處理結果等資訊。</t>
+  </si>
+  <si>
+    <t>是否提供足夠資源，使日誌保存不致造成系統資源匱乏？</t>
+  </si>
+  <si>
+    <t>計畫導入日誌系統後，使用RotatingFileHandler進行日誌輪替(每個檔桡8朂10MB，保留10個備份)。</t>
+  </si>
+  <si>
+    <t>目前無日誌監控。計畫導入日誌系統後，透過系統監控工具檢查日誌寫入狀態。</t>
+  </si>
+  <si>
+    <t>系統時間由作業系統NTP服務統一校時，無需應用程式層級實作。</t>
+  </si>
+  <si>
+    <t>目前無自動化資料刪除機制。計畫下個版本實作自動化資料清理功能，可設定任務記錄保存期限5年)。</t>
+  </si>
+  <si>
+    <t>是否建立單一存取路徑，防止非授權使用者從不同管道進入系統？</t>
+  </si>
+  <si>
+    <t>透過防火牆與內網隔離，僅允許特定網段透過Web介面存取。系統部署於特定裝置，控制存取路徑。</t>
+  </si>
+  <si>
+    <t>是否建立足夠之安全連線機制，如TLS.1.2以上？</t>
+  </si>
+  <si>
+    <t>目前使用HTTP協定，僅於內部網路運作。計畫未來版本透過反向代理(Nginx)配置TLS 1.3加密傳輸。</t>
+  </si>
+  <si>
+    <t>是否根據上述需求分析及架構設計評估，並回饋其安全需求修正？</t>
+  </si>
+  <si>
+    <t>已根據功能需求完成系統開發，並透過使用者回駈持續優化。</t>
+  </si>
+  <si>
+    <t>是否根據將上述需求分析及架構設計文件化，並留存相關記錄？</t>
+  </si>
+  <si>
+    <t>提供完整文件，包含README.md(使用說明)、CLAUDE.md(架構與開發指引)、BATCH_TASKS_README.md(批次處理說明)等，並透過Git版控管理。</t>
+  </si>
+  <si>
+    <t>小型內部工具，開發與生產環境相同。透過Git分支(main/develop)實現邏輯區隔。未來若資源允許將建立獨立測試環境。</t>
+  </si>
+  <si>
+    <t>小型內部工具，開發與測試由同一團隊負責。透過Git版控管理變更，確保可追溯性。</t>
+  </si>
+  <si>
+    <t>目前無正式安全測試流程。建議導入靜態分析工具(bandit)與依賴漏洞掃描(pip-audit)，定期進行基本安全檢測。</t>
+  </si>
+  <si>
+    <t>是否通知妥託單位測試，並製作系統測試報告（包含功能性及安全性測試結果），並控管相關文件紀錄？</t>
+  </si>
+  <si>
+    <t>目前無正式測試報告。建議建立基本測試流程，包含功能測試與安全掃描，並記錄測試結果。</t>
+  </si>
+  <si>
+    <t>是否制定系統測試若需要真實資料之申請程序與如何取得，並留存相關紀錄？</t>
+  </si>
+  <si>
+    <t>測試不使用真實資料，使用範例文件即可完成功能驗證，不需要申請程序。</t>
+  </si>
+  <si>
+    <t>若上述為個資等敏感資訊之取得，是否已經去識別化等處理措施？</t>
+  </si>
+  <si>
+    <t>測試不使用真實個資，不需去識別化處理。</t>
+  </si>
+  <si>
+    <t>使用SQLite資料庫，圖片以Base64編碼儲存。未來可考慮導入資料庫加密(SQLCipher)提升安全性。</t>
+  </si>
+  <si>
+    <t>若架構涉及系統間之資料交換，是否具安全的傳輸機制？</t>
+  </si>
+  <si>
+    <t>PaddleOCR主服務透過HTTP調用CLIP服務(Port 8081)。兩個服務部署於同一主機或內網，透過防火牆隔離外部存取。</t>
+  </si>
+  <si>
+    <t>若以API進行資料交換，是否具備安全的認證機制？如採取憑證或HASH過之密碼存放於config檔</t>
+  </si>
+  <si>
+    <t>目前無正式弱點修補流程。建議導入依賴漏洞掃描工具(pip-audit)，定期檢查並更新套件，修補已知漏洞。</t>
+  </si>
+  <si>
+    <t>小型內部工具，透過Git分支管理實現邏輯區隔。未來若資源允許將建立獨立測試環境。</t>
+  </si>
+  <si>
+    <t>小型內部工具，開發、部署、維護由同一團隊負責。透過Git版控確保變更可追溯。</t>
+  </si>
+  <si>
+    <t>是否制定系統版本發佈與更新程序，並留存相關紀錄？</t>
+  </si>
+  <si>
+    <t>透過Git進行版本管理，使用語意化版本號。更新流程:開發分支測試→合併至主分支→重新部署服務。所有變更記錄於Git commit歷史。</t>
+  </si>
+  <si>
+    <t>是否針對委託單位之相關人員，進行系統操作與安全教育訓練？</t>
+  </si>
+  <si>
+    <t>目前無正式教育訓練。建議編寫使用者操作手冊，包含系統操作說明與安全注意事項，並於系統上線前進行操作示範。</t>
+  </si>
+  <si>
+    <t>是否根據各項變更之需求，重複上述3~4流程已確認變更作業程序，並留存相關紀錄？</t>
+  </si>
+  <si>
+    <t>透過Git版控管理所有變更，每次更新均記錄commit訊息。重大變更需進行功能測試後再部署。系統變更遍循3-4階段流程。</t>
+  </si>
+  <si>
+    <t>進行上述變更作業，是否對既有系統備份，並留存相關紀錄？</t>
+  </si>
+  <si>
+    <t>每次更新前會備份SQLite資料庫檔案(batch_tasks.db、ocr_tasks.db)，並透過Git保存歷史版本。備份記錄保存於指定目錄。</t>
+  </si>
+  <si>
+    <t>若為硬體擴充或虛擬化，是否重複上述3~4流程已確認變更作業程序，並留存相關紀錄？</t>
+  </si>
+  <si>
+    <t>無硬體擴充需求，系統可部署於現有工作站或伺服器。若需擴充資源則遍循3-4階段流程進行評估。</t>
+  </si>
+  <si>
+    <t>是否定期依法將過期之資料刪除，並留下刪除之記路？如個資保存期限</t>
+  </si>
+  <si>
+    <t>目前無自動化資料刪除機制。管理者可手動刪除舊任務釋放空間。建議實作自動化資料清理功能，可設定保存期限5年)。</t>
+  </si>
+  <si>
+    <t>是否依規定將資料備份或銷燬，並依據資料安全性等級保存於規定的環境，並留存相關記錄？</t>
+  </si>
+  <si>
+    <t>已制定系統下線程序:1.匯出所有資料庫內容為SQL或Excel格式 2.備份資料庫檔案至指定位置 3.清理暫存目錄(output/，temp_ocr/) 4.若涉及機敏資料，使用安全刪除工具徹底清除。留存下線記錄。</t>
+  </si>
+  <si>
+    <t>資料庫記錄任務歷史，可追溯處理記錄。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>程式碼透過Git版控管理，資料儲存於SQLite資料庫，定期備份.db檔案。若系統故障可於1小時內復原。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>無登入通知機制。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已實作應用程式日誌功能。使用Python logging模組記錄檔案上傳、OCR執行、批次任務等操作。日誌儲存於 logs/ 目錄,使用RotatingFileHandler輪替(10MB/檔,保疑10個備份),可追溯90天操作記錄。</t>
+  </si>
+  <si>
+    <t>已實作應用程式日誌系統,記錄保存90天。若未來處理個資,將延長至5年以符合法規要求。</t>
+  </si>
+  <si>
+    <t>日誌包含: 時間戳記、事件類型(INFO/WARNING/ERROR)、檔案位置、任務ID、檔案名稱、處理結果、錯誤訊息等資訊。</t>
+  </si>
+  <si>
+    <t>使用RotatingFileHandler進行日誌輪替,每個檔栘8朂10MB,保疑10個備份檔,總容量100MB,不會造成系統資源匪乏。</t>
+  </si>
+  <si>
+    <t>目前無日誌失效監控機制。建議未來整合系統監控工具(如Prometheus)監控日誌寫入狀態。</t>
+  </si>
+  <si>
+    <t>已導入安全測試工具: bandit(靜態程式碼分析)、pip-audit(依賴漏洞掃描)。提供security_check.py自動化檢測腳本。報告儲存於 security_reports/ 目錄。</t>
+  </si>
+  <si>
+    <t>已建立安全測試流程與文件(SECURITY_TESTING.md)。包含功能測試與安全掃描指引。建議定期執行安全檢測(每週/每月)。</t>
+  </si>
+  <si>
+    <t>已導入pip-audit依賴漏洞掃描工具,可定期檢查並更新套件以修補已知漏洞。建議每月執行一次完整檢測。</t>
+  </si>
+  <si>
+    <t>已編寫完整的使用者操作手冊(USER_MANUAL.md),包含系統操作說明、安全注意事項、常見問題與故障排除。建議於系統上線前進行30-60分鐘操作示範。</t>
   </si>
 </sst>
 </file>
@@ -761,9 +767,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -801,9 +807,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -836,26 +842,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -888,26 +877,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1083,8 +1055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="true" zoomScale="134" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="true" topLeftCell="A21" zoomScale="134" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
@@ -1093,13 +1065,13 @@
     <col customWidth="true" max="2" min="2" style="1" width="47.375"/>
     <col customWidth="true" max="4" min="3" width="7.125"/>
     <col customWidth="true" max="5" min="5" width="8.125"/>
-    <col customWidth="true" max="6" min="6" width="22.5"/>
+    <col customWidth="true" max="6" min="6" width="128.625"/>
     <col customWidth="true" max="7" min="7" width="14.375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24">
       <c r="A1" s="19" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -1109,27 +1081,27 @@
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="true">
       <c r="A2" s="5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="15" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B3" s="16"/>
       <c r="C3" s="17"/>
@@ -1142,15 +1114,19 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D4" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E4" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F4" s="12" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1158,15 +1134,19 @@
         <v>1.2</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D5" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E5" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F5" s="12" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1174,15 +1154,19 @@
         <v>1.3</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="D6" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F6" s="11" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1190,15 +1174,19 @@
         <v>1.4</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D7" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E7" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="F7" s="3" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1206,15 +1194,19 @@
         <v>1.5</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="2"/>
+        <v>57</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D8" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E8" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="F8" s="11" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1222,15 +1214,19 @@
         <v>1.6</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D9" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E9" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="F9" s="11" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1238,15 +1234,19 @@
         <v>1.7</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F10" s="11" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1254,15 +1254,19 @@
         <v>1.8</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="D11" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E11" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F11" s="11" t="s">
-        <v>97</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1270,36 +1274,44 @@
         <v>1.9</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D12" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E12" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="F12" s="11" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="9" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="D13" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E13" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F13" s="11" t="s">
-        <v>99</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="15" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B14" s="16"/>
       <c r="C14" s="17"/>
@@ -1307,20 +1319,24 @@
       <c r="E14" s="17"/>
       <c r="F14" s="18"/>
     </row>
-    <row r="15" spans="1:6" ht="31.5">
+    <row r="15" spans="1:6" ht="63">
       <c r="A15" s="9">
         <v>2.1</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D15" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E15" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="F15" s="14" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1328,15 +1344,19 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D16" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E16" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="F16" s="11" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1344,15 +1364,19 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D17" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E17" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="F17" s="11" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="31.5">
@@ -1360,15 +1384,19 @@
         <v>2.4</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" s="2"/>
+        <v>54</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D18" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E18" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="F18" s="11" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="31.5">
@@ -1376,15 +1404,19 @@
         <v>2.5</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="D19" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E19" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F19" s="11" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="31.5">
@@ -1392,15 +1424,19 @@
         <v>2.6</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="D20" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E20" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F20" s="11" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="31.5">
@@ -1408,15 +1444,19 @@
         <v>2.7</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="D21" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E21" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F21" s="11" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1424,15 +1464,19 @@
         <v>2.8</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D22" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E22" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F22" s="11" t="s">
-        <v>107</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="31.5">
@@ -1440,84 +1484,104 @@
         <v>2.9</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="D23" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E23" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F23" s="11" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="31.5">
       <c r="A24" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D24" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="11" t="s">
         <v>89</v>
-      </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="11" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="31.5">
       <c r="A25" s="9" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F25" s="11" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="31.5">
       <c r="A26" s="9" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="2"/>
+        <v>90</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="D26" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E26" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F26" s="11" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="9" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="2"/>
+        <v>92</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D27" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E27" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F27" s="11" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="15" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="17"/>
@@ -1527,183 +1591,227 @@
     </row>
     <row r="29" spans="1:6" ht="31.5">
       <c r="A29" s="9" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>37</v>
+        <v>94</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F29" s="12" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="31.5">
       <c r="A30" s="9" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F30" s="12" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="9" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D31" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E31" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="F31" s="3" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="9" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D32" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E32" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="F32" s="3" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="31.5">
       <c r="A33" s="9" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C33" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="D33" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E33" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F33" s="3" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="31.5">
       <c r="A34" s="9" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="D34" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E34" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F34" s="3" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="31.5">
       <c r="A35" s="9" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
+        <v>103</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="E35" s="2" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="31.5">
       <c r="A36" s="9" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
+        <v>105</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="E36" s="2" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="9" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="E37" s="2" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="31.5">
       <c r="A38" s="9" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F38" s="3" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="31.5">
       <c r="A39" s="9" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F39" s="3" t="s">
-        <v>121</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="16.5" customHeight="true">
       <c r="A40" s="15" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B40" s="16"/>
       <c r="C40" s="17"/>
@@ -1713,103 +1821,127 @@
     </row>
     <row r="41" spans="1:6" ht="16.5" customHeight="true">
       <c r="A41" s="9" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C41" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="D41" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E41" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F41" s="12" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C42" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D42" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E42" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="F42" s="3" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="31.5">
       <c r="A43" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C43" s="2"/>
+      <c r="C43" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D43" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E43" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="F43" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="31.5">
       <c r="A44" s="9" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F44" s="3" t="s">
-        <v>124</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="31.5">
       <c r="A45" s="9" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>2</v>
+        <v>114</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F45" s="3" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="31.5">
       <c r="A46" s="9" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" s="2"/>
+        <v>116</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="D46" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E46" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F46" s="3" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="16.5" customHeight="true">
       <c r="A47" s="15" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="B47" s="16"/>
       <c r="C47" s="17"/>
@@ -1819,71 +1951,87 @@
     </row>
     <row r="48" spans="1:6" ht="31.5">
       <c r="A48" s="9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>68</v>
+        <v>118</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F48" s="3" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="31.5">
       <c r="A49" s="9" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F49" s="3" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="31.5">
       <c r="A50" s="9" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
+        <v>122</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="E50" s="2" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="31.5">
       <c r="A51" s="9" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C51" s="2"/>
+        <v>124</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D51" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E51" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F51" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="15" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="B52" s="16"/>
       <c r="C52" s="17"/>
@@ -1893,18 +2041,22 @@
     </row>
     <row r="53" spans="1:6" ht="31.5">
       <c r="A53" s="9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C53" s="2"/>
+        <v>126</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="D53" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E53" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F53" s="12" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>